<commit_message>
Criando arquivo para gerar os dados de inderencia como um arquivo separado: modelo_interativo_NGE
</commit_message>
<xml_diff>
--- a/testes/resultado_inferência_NGE.xlsx
+++ b/testes/resultado_inferência_NGE.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet_name_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inferencia por IA" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,27 +462,27 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>qtd_pag_word</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
           <t>qtd_carc</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>qtd_tabela</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>qtd_image</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>qtd_estilos</t>
+        </is>
+      </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>qtd_estilos</t>
+          <t>qtd_pag_word</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>QTD_PAG_INVERIDO</t>
+          <t>QTD_PAG_INFERIDO</t>
         </is>
       </c>
     </row>
@@ -516,19 +516,19 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
+        <v>70983</v>
+      </c>
+      <c r="H2" t="n">
+        <v>288</v>
+      </c>
+      <c r="I2" t="n">
+        <v>211</v>
+      </c>
+      <c r="J2" t="n">
+        <v>16</v>
+      </c>
+      <c r="K2" t="n">
         <v>34</v>
-      </c>
-      <c r="H2" t="n">
-        <v>70983</v>
-      </c>
-      <c r="I2" t="n">
-        <v>288</v>
-      </c>
-      <c r="J2" t="n">
-        <v>211</v>
-      </c>
-      <c r="K2" t="n">
-        <v>16</v>
       </c>
       <c r="L2" t="n">
         <v>48</v>
@@ -557,19 +557,19 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
+        <v>23238</v>
+      </c>
+      <c r="H3" t="n">
+        <v>133</v>
+      </c>
+      <c r="I3" t="n">
+        <v>107</v>
+      </c>
+      <c r="J3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K3" t="n">
         <v>30</v>
-      </c>
-      <c r="H3" t="n">
-        <v>23238</v>
-      </c>
-      <c r="I3" t="n">
-        <v>133</v>
-      </c>
-      <c r="J3" t="n">
-        <v>107</v>
-      </c>
-      <c r="K3" t="n">
-        <v>29</v>
       </c>
       <c r="L3" t="n">
         <v>48</v>
@@ -598,19 +598,19 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
+        <v>87223</v>
+      </c>
+      <c r="H4" t="n">
+        <v>275</v>
+      </c>
+      <c r="I4" t="n">
+        <v>156</v>
+      </c>
+      <c r="J4" t="n">
+        <v>127</v>
+      </c>
+      <c r="K4" t="n">
         <v>68</v>
-      </c>
-      <c r="H4" t="n">
-        <v>87223</v>
-      </c>
-      <c r="I4" t="n">
-        <v>275</v>
-      </c>
-      <c r="J4" t="n">
-        <v>156</v>
-      </c>
-      <c r="K4" t="n">
-        <v>127</v>
       </c>
       <c r="L4" t="n">
         <v>98</v>
@@ -639,19 +639,19 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
+        <v>17783</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>23</v>
+      </c>
+      <c r="K5" t="n">
         <v>26</v>
-      </c>
-      <c r="H5" t="n">
-        <v>17783</v>
-      </c>
-      <c r="I5" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" t="n">
-        <v>23</v>
       </c>
       <c r="L5" t="n">
         <v>48</v>
@@ -680,19 +680,19 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
+        <v>14560</v>
+      </c>
+      <c r="H6" t="n">
+        <v>260</v>
+      </c>
+      <c r="I6" t="n">
+        <v>142</v>
+      </c>
+      <c r="J6" t="n">
+        <v>28</v>
+      </c>
+      <c r="K6" t="n">
         <v>23</v>
-      </c>
-      <c r="H6" t="n">
-        <v>14560</v>
-      </c>
-      <c r="I6" t="n">
-        <v>260</v>
-      </c>
-      <c r="J6" t="n">
-        <v>142</v>
-      </c>
-      <c r="K6" t="n">
-        <v>28</v>
       </c>
       <c r="L6" t="n">
         <v>46</v>
@@ -721,19 +721,19 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
+        <v>14344</v>
+      </c>
+      <c r="H7" t="n">
+        <v>277</v>
+      </c>
+      <c r="I7" t="n">
+        <v>158</v>
+      </c>
+      <c r="J7" t="n">
+        <v>29</v>
+      </c>
+      <c r="K7" t="n">
         <v>22</v>
-      </c>
-      <c r="H7" t="n">
-        <v>14344</v>
-      </c>
-      <c r="I7" t="n">
-        <v>277</v>
-      </c>
-      <c r="J7" t="n">
-        <v>158</v>
-      </c>
-      <c r="K7" t="n">
-        <v>29</v>
       </c>
       <c r="L7" t="n">
         <v>46</v>
@@ -762,19 +762,19 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
+        <v>12344</v>
+      </c>
+      <c r="H8" t="n">
+        <v>258</v>
+      </c>
+      <c r="I8" t="n">
+        <v>140</v>
+      </c>
+      <c r="J8" t="n">
+        <v>25</v>
+      </c>
+      <c r="K8" t="n">
         <v>20</v>
-      </c>
-      <c r="H8" t="n">
-        <v>12344</v>
-      </c>
-      <c r="I8" t="n">
-        <v>258</v>
-      </c>
-      <c r="J8" t="n">
-        <v>140</v>
-      </c>
-      <c r="K8" t="n">
-        <v>25</v>
       </c>
       <c r="L8" t="n">
         <v>46</v>
@@ -803,19 +803,19 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
+        <v>247205</v>
+      </c>
+      <c r="H9" t="n">
+        <v>154</v>
+      </c>
+      <c r="I9" t="n">
+        <v>130</v>
+      </c>
+      <c r="J9" t="n">
+        <v>26</v>
+      </c>
+      <c r="K9" t="n">
         <v>142</v>
-      </c>
-      <c r="H9" t="n">
-        <v>247205</v>
-      </c>
-      <c r="I9" t="n">
-        <v>154</v>
-      </c>
-      <c r="J9" t="n">
-        <v>130</v>
-      </c>
-      <c r="K9" t="n">
-        <v>26</v>
       </c>
       <c r="L9" t="n">
         <v>198</v>
@@ -844,19 +844,19 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
+        <v>97635</v>
+      </c>
+      <c r="H10" t="n">
+        <v>126</v>
+      </c>
+      <c r="I10" t="n">
+        <v>94</v>
+      </c>
+      <c r="J10" t="n">
+        <v>54</v>
+      </c>
+      <c r="K10" t="n">
         <v>75</v>
-      </c>
-      <c r="H10" t="n">
-        <v>97635</v>
-      </c>
-      <c r="I10" t="n">
-        <v>126</v>
-      </c>
-      <c r="J10" t="n">
-        <v>94</v>
-      </c>
-      <c r="K10" t="n">
-        <v>54</v>
       </c>
       <c r="L10" t="n">
         <v>110</v>
@@ -885,19 +885,19 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
+        <v>75538</v>
+      </c>
+      <c r="H11" t="n">
+        <v>131</v>
+      </c>
+      <c r="I11" t="n">
+        <v>98</v>
+      </c>
+      <c r="J11" t="n">
+        <v>21</v>
+      </c>
+      <c r="K11" t="n">
         <v>38</v>
-      </c>
-      <c r="H11" t="n">
-        <v>75538</v>
-      </c>
-      <c r="I11" t="n">
-        <v>131</v>
-      </c>
-      <c r="J11" t="n">
-        <v>98</v>
-      </c>
-      <c r="K11" t="n">
-        <v>21</v>
       </c>
       <c r="L11" t="n">
         <v>68</v>
@@ -926,19 +926,19 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
+        <v>72824</v>
+      </c>
+      <c r="H12" t="n">
+        <v>262</v>
+      </c>
+      <c r="I12" t="n">
+        <v>144</v>
+      </c>
+      <c r="J12" t="n">
+        <v>16</v>
+      </c>
+      <c r="K12" t="n">
         <v>48</v>
-      </c>
-      <c r="H12" t="n">
-        <v>72824</v>
-      </c>
-      <c r="I12" t="n">
-        <v>262</v>
-      </c>
-      <c r="J12" t="n">
-        <v>144</v>
-      </c>
-      <c r="K12" t="n">
-        <v>16</v>
       </c>
       <c r="L12" t="n">
         <v>75</v>
@@ -967,19 +967,19 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
+        <v>72613</v>
+      </c>
+      <c r="H13" t="n">
+        <v>286</v>
+      </c>
+      <c r="I13" t="n">
+        <v>207</v>
+      </c>
+      <c r="J13" t="n">
+        <v>15</v>
+      </c>
+      <c r="K13" t="n">
         <v>45</v>
-      </c>
-      <c r="H13" t="n">
-        <v>72613</v>
-      </c>
-      <c r="I13" t="n">
-        <v>286</v>
-      </c>
-      <c r="J13" t="n">
-        <v>207</v>
-      </c>
-      <c r="K13" t="n">
-        <v>15</v>
       </c>
       <c r="L13" t="n">
         <v>70</v>
@@ -1008,19 +1008,19 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
+        <v>163469</v>
+      </c>
+      <c r="H14" t="n">
+        <v>12</v>
+      </c>
+      <c r="I14" t="n">
+        <v>65</v>
+      </c>
+      <c r="J14" t="n">
+        <v>15</v>
+      </c>
+      <c r="K14" t="n">
         <v>81</v>
-      </c>
-      <c r="H14" t="n">
-        <v>163469</v>
-      </c>
-      <c r="I14" t="n">
-        <v>12</v>
-      </c>
-      <c r="J14" t="n">
-        <v>65</v>
-      </c>
-      <c r="K14" t="n">
-        <v>15</v>
       </c>
       <c r="L14" t="n">
         <v>114</v>
@@ -1049,19 +1049,19 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
+        <v>660609</v>
+      </c>
+      <c r="H15" t="n">
+        <v>107</v>
+      </c>
+      <c r="I15" t="n">
+        <v>75</v>
+      </c>
+      <c r="J15" t="n">
+        <v>27</v>
+      </c>
+      <c r="K15" t="n">
         <v>424</v>
-      </c>
-      <c r="H15" t="n">
-        <v>660609</v>
-      </c>
-      <c r="I15" t="n">
-        <v>107</v>
-      </c>
-      <c r="J15" t="n">
-        <v>75</v>
-      </c>
-      <c r="K15" t="n">
-        <v>27</v>
       </c>
       <c r="L15" t="n">
         <v>460</v>
@@ -1090,19 +1090,19 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
+        <v>586948</v>
+      </c>
+      <c r="H16" t="n">
+        <v>256</v>
+      </c>
+      <c r="I16" t="n">
+        <v>138</v>
+      </c>
+      <c r="J16" t="n">
+        <v>21</v>
+      </c>
+      <c r="K16" t="n">
         <v>373</v>
-      </c>
-      <c r="H16" t="n">
-        <v>586948</v>
-      </c>
-      <c r="I16" t="n">
-        <v>256</v>
-      </c>
-      <c r="J16" t="n">
-        <v>138</v>
-      </c>
-      <c r="K16" t="n">
-        <v>21</v>
       </c>
       <c r="L16" t="n">
         <v>420</v>
@@ -1131,19 +1131,19 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
+        <v>22781</v>
+      </c>
+      <c r="H17" t="n">
+        <v>279</v>
+      </c>
+      <c r="I17" t="n">
+        <v>160</v>
+      </c>
+      <c r="J17" t="n">
+        <v>20</v>
+      </c>
+      <c r="K17" t="n">
         <v>29</v>
-      </c>
-      <c r="H17" t="n">
-        <v>22781</v>
-      </c>
-      <c r="I17" t="n">
-        <v>279</v>
-      </c>
-      <c r="J17" t="n">
-        <v>160</v>
-      </c>
-      <c r="K17" t="n">
-        <v>20</v>
       </c>
       <c r="L17" t="n">
         <v>48</v>
@@ -1172,19 +1172,19 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
+        <v>33141</v>
+      </c>
+      <c r="H18" t="n">
+        <v>293</v>
+      </c>
+      <c r="I18" t="n">
+        <v>216</v>
+      </c>
+      <c r="J18" t="n">
+        <v>19</v>
+      </c>
+      <c r="K18" t="n">
         <v>24</v>
-      </c>
-      <c r="H18" t="n">
-        <v>33141</v>
-      </c>
-      <c r="I18" t="n">
-        <v>293</v>
-      </c>
-      <c r="J18" t="n">
-        <v>216</v>
-      </c>
-      <c r="K18" t="n">
-        <v>19</v>
       </c>
       <c r="L18" t="n">
         <v>48</v>

</xml_diff>